<commit_message>
working xlsx read and template generation
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryvecchione/Desktop/Home/myboathouse2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E75033F-EB32-D941-8707-694028117287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057B6B0B-0400-FF46-9669-C8B9F8DEDE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{6D2E25F7-B84A-894E-A3F5-C6C51AF1EF79}"/>
+    <workbookView xWindow="8460" yWindow="4200" windowWidth="28040" windowHeight="17440" xr2:uid="{6D2E25F7-B84A-894E-A3F5-C6C51AF1EF79}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
     <sheet name="Roster" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -481,7 +480,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>